<commit_message>
Clean up repo: removed .DS_store
</commit_message>
<xml_diff>
--- a/AR_Template_API.xlsx
+++ b/AR_Template_API.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhubb/Documents/ar_excel_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F273FC9B-67C1-3A46-A628-9FE9410F09F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E204970-92AC-864C-BDB9-AFBBC752C758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12280" yWindow="500" windowWidth="16520" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10520" yWindow="500" windowWidth="17580" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sheet" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>